<commit_message>
Models create to database
</commit_message>
<xml_diff>
--- a/sql/estrutura e ordem CRUD.xlsx
+++ b/sql/estrutura e ordem CRUD.xlsx
@@ -607,6 +607,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
@@ -638,6 +641,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -663,6 +669,9 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -688,6 +697,9 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
@@ -791,6 +803,9 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -821,6 +836,9 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -869,6 +887,9 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -910,6 +931,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -946,6 +970,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -1010,6 +1037,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -1075,6 +1105,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -1160,6 +1193,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -1227,6 +1263,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -1276,6 +1315,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -1316,6 +1358,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>

</xml_diff>